<commit_message>
Added gets better the algorithm cells
</commit_message>
<xml_diff>
--- a/code/results_cellsMejorado/final/results_100(1).xlsx
+++ b/code/results_cellsMejorado/final/results_100(1).xlsx
@@ -508,10 +508,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -522,7 +522,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>272386830</v>
+        <v>47581786</v>
       </c>
       <c r="C3" s="3">
         <v>49094.7221568628</v>
@@ -536,7 +536,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>5.690386402e+18</v>
+        <v>7.659198175e+16</v>
       </c>
       <c r="C4" s="2">
         <v>1.308599303e+19</v>
@@ -550,7 +550,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>102344.562</v>
+        <v>98410.14599999999</v>
       </c>
       <c r="C5" s="3">
         <v>3481.0788823529</v>
@@ -564,7 +564,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>132.65249</v>
+        <v>112.73258</v>
       </c>
       <c r="C6" s="3">
         <v>84.30386294119999</v>
@@ -578,7 +578,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>119.69693</v>
+        <v>88.67249200000001</v>
       </c>
       <c r="C7" s="2">
         <v>201.4980607843</v>
@@ -592,7 +592,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>4.8452392</v>
+        <v>2.824631</v>
       </c>
       <c r="C8" s="2">
         <v>6.3202614647</v>
@@ -606,7 +606,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>213.73985</v>
+        <v>161.83235</v>
       </c>
       <c r="C9" s="2">
         <v>233.4221882353</v>
@@ -620,7 +620,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="3">
-        <v>111.304962</v>
+        <v>92.32836</v>
       </c>
       <c r="C10" s="2">
         <v>189.3719607843</v>
@@ -634,7 +634,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="2">
-        <v>772.95628</v>
+        <v>605.33724</v>
       </c>
       <c r="C11" s="3">
         <v>65.2973029608</v>
@@ -648,7 +648,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="3">
-        <v>3495.9154</v>
+        <v>2073.373</v>
       </c>
       <c r="C12" s="2">
         <v>3763.561372549</v>
@@ -662,7 +662,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="2">
-        <v>1011.09</v>
+        <v>674.1830200000001</v>
       </c>
       <c r="C13" s="3">
         <v>79.5827970588</v>
@@ -676,7 +676,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="2">
-        <v>42261656</v>
+        <v>12001323.8</v>
       </c>
       <c r="C14" s="3">
         <v>325765.1509803921</v>
@@ -690,7 +690,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="2">
-        <v>45610997</v>
+        <v>10937070</v>
       </c>
       <c r="C15" s="3">
         <v>153.6136039216</v>
@@ -704,7 +704,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="2">
-        <v>362255.35</v>
+        <v>341142.92</v>
       </c>
       <c r="C16" s="3">
         <v>71.0022382353</v>
@@ -718,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="2">
-        <v>7802708</v>
+        <v>806677.05</v>
       </c>
       <c r="C17" s="3">
         <v>62.5567343137</v>
@@ -732,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="3">
-        <v>1078.39229</v>
+        <v>926.81639</v>
       </c>
       <c r="C18" s="2">
         <v>1319.2334901961</v>
@@ -746,7 +746,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="3">
-        <v>322.15652</v>
+        <v>362.91416</v>
       </c>
       <c r="C19" s="2">
         <v>480.8806464706</v>
@@ -760,7 +760,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="2">
-        <v>1115853.12</v>
+        <v>671618.5699999999</v>
       </c>
       <c r="C20" s="3">
         <v>61.2224523529</v>
@@ -774,7 +774,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="2">
-        <v>10444793.1</v>
+        <v>2568815</v>
       </c>
       <c r="C21" s="3">
         <v>35.7226817647</v>
@@ -787,10 +787,10 @@
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2">
-        <v>472.27617</v>
-      </c>
-      <c r="C22" s="3">
+      <c r="B22" s="3">
+        <v>238.2233</v>
+      </c>
+      <c r="C22" s="2">
         <v>275.1128247059</v>
       </c>
       <c r="D22" s="2">
@@ -802,7 +802,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="3">
-        <v>253.2834</v>
+        <v>235.40831</v>
       </c>
       <c r="C23" s="2">
         <v>325.4940980392</v>
@@ -816,7 +816,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="2">
-        <v>198.49614</v>
+        <v>137.92548</v>
       </c>
       <c r="C24" s="3">
         <v>100.2234960784</v>
@@ -830,7 +830,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="3">
-        <v>428.9448</v>
+        <v>431.40883</v>
       </c>
       <c r="C25" s="2">
         <v>534.6091764706</v>
@@ -844,7 +844,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="3">
-        <v>549.6828</v>
+        <v>487.85666</v>
       </c>
       <c r="C26" s="2">
         <v>605.9018411765001</v>
@@ -858,7 +858,7 @@
         <v>28</v>
       </c>
       <c r="B27" s="2">
-        <v>419.84425</v>
+        <v>412.19445</v>
       </c>
       <c r="C27" s="3">
         <v>387.027972549</v>
@@ -872,7 +872,7 @@
         <v>29</v>
       </c>
       <c r="B28" s="2">
-        <v>670.1601899999999</v>
+        <v>435.87083</v>
       </c>
       <c r="C28" s="3">
         <v>403.7672980392</v>
@@ -886,7 +886,7 @@
         <v>30</v>
       </c>
       <c r="B29" s="2">
-        <v>538.57406</v>
+        <v>529.1650100000001</v>
       </c>
       <c r="C29" s="3">
         <v>492.5197803922</v>
@@ -900,7 +900,7 @@
         <v>31</v>
       </c>
       <c r="B30" s="2">
-        <v>468.92089</v>
+        <v>455.38336</v>
       </c>
       <c r="C30" s="3">
         <v>394.2695647059</v>
@@ -914,7 +914,7 @@
         <v>32</v>
       </c>
       <c r="B31" s="3">
-        <v>756.57375</v>
+        <v>596.36086</v>
       </c>
       <c r="C31" s="2">
         <v>1025.0945705882</v>
@@ -928,7 +928,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="2">
-        <v>2693751.27</v>
+        <v>1430768.39</v>
       </c>
       <c r="C32" s="2">
         <v>3656.5519411765</v>

</xml_diff>